<commit_message>
Added TestNBA and TestBasePage class. Also added data in espn_data excel file
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espn_data.xlsx
+++ b/com.espn/src/test/resources/espn_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26333F45-69F3-40BD-92DD-5607B35CA273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FD84FB-6141-4BEC-A468-AE28B9F00229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -32,6 +32,197 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Celtics</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Nets</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Golden State</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Oklahoma City</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Knicks</t>
+  </si>
+  <si>
+    <t>76ers</t>
+  </si>
+  <si>
+    <t>Raptors</t>
+  </si>
+  <si>
+    <t>Nuggets</t>
+  </si>
+  <si>
+    <t>Timberwolves</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Trail Blazers</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>Bulls</t>
+  </si>
+  <si>
+    <t>Cavaliers</t>
+  </si>
+  <si>
+    <t>Pistons</t>
+  </si>
+  <si>
+    <t>Pacers</t>
+  </si>
+  <si>
+    <t>Bucks</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>Clippers</t>
+  </si>
+  <si>
+    <t>Lakers</t>
+  </si>
+  <si>
+    <t>Suns</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Hawks</t>
+  </si>
+  <si>
+    <t>Hornets</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Wizards</t>
+  </si>
+  <si>
+    <t>Mavericks</t>
+  </si>
+  <si>
+    <t>Rockets</t>
+  </si>
+  <si>
+    <t>Grizzlies</t>
+  </si>
+  <si>
+    <t>Pelicans</t>
+  </si>
+  <si>
+    <t>Spurs</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,9 +256,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,15 +574,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
setting up BMWUSA module for test cases
</commit_message>
<xml_diff>
--- a/com.espn/src/test/resources/espn_data.xlsx
+++ b/com.espn/src/test/resources/espn_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.espn\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FD84FB-6141-4BEC-A468-AE28B9F00229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1EB845-E4DF-481C-9C50-5ABF21CFC6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="nbaTeams" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -577,7 +578,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,4 +839,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>